<commit_message>
SF User list changes - 16 May - Initial
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTI0045469_VerifyNewTitleAddedinTitleRateSheet.xlsx
+++ b/TestData/LV_TMTI0045469_VerifyNewTitleAddedinTitleRateSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8851AD-A2AA-4734-A86E-2E776DA38FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E356F749-E4E7-40B6-B7D4-53717215A2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -69,22 +69,22 @@
     <t>HL Banker</t>
   </si>
   <si>
-    <t>Ashley Choi</t>
-  </si>
-  <si>
     <t>Profile</t>
   </si>
   <si>
     <t>UserGroupName</t>
   </si>
   <si>
-    <t xml:space="preserve">Time Tracking Litigation Supervisor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supervisor </t>
-  </si>
-  <si>
     <t>1000</t>
+  </si>
+  <si>
+    <t>Amy Xia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time Tracking Litigation </t>
+  </si>
+  <si>
+    <t>CF Financial User</t>
   </si>
 </sst>
 </file>
@@ -416,36 +416,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -462,17 +462,17 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -490,17 +490,17 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -514,20 +514,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC3538F-EBF7-4442-B955-CB25CC734266}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -541,7 +541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -549,7 +549,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>

</xml_diff>